<commit_message>
Added ScrapedData3 - with owner name, and full Improv/Land/Total for current and previous Appraised & Assessed
</commit_message>
<xml_diff>
--- a/84 & 92 Orford Road-11Jan2022.xlsx
+++ b/84 & 92 Orford Road-11Jan2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richb/Documents/Projects/Tax Fairness in Lyme/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896A21D3-3AD7-784E-A4FE-718CEE5FDBEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB8CB84-C568-0C45-9E6B-022830594EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8020" yWindow="460" windowWidth="15560" windowHeight="13680" xr2:uid="{24FE3324-035D-CA45-AC6C-ED3F3972A86E}"/>
+    <workbookView xWindow="280" yWindow="1360" windowWidth="15560" windowHeight="13680" xr2:uid="{24FE3324-035D-CA45-AC6C-ED3F3972A86E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="29">
   <si>
     <t>Improvements</t>
   </si>
@@ -107,6 +107,18 @@
   </si>
   <si>
     <t>Properties by Post Pond in Lyme NH</t>
+  </si>
+  <si>
+    <t>408/19</t>
+  </si>
+  <si>
+    <t>408/20</t>
+  </si>
+  <si>
+    <t>408/22.1000</t>
+  </si>
+  <si>
+    <t>408/22.2000</t>
   </si>
 </sst>
 </file>
@@ -482,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE8F50C-D361-254A-AD5F-93A5346E20DB}">
   <dimension ref="A1:J93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1605,6 +1617,9 @@
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="B56" s="1" t="s">
         <v>8</v>
       </c>
@@ -1785,6 +1800,9 @@
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="B64" s="1" t="s">
         <v>8</v>
       </c>
@@ -1960,6 +1978,9 @@
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="B72" s="1" t="s">
         <v>8</v>
       </c>
@@ -2134,6 +2155,9 @@
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="B80" s="1" t="s">
         <v>8</v>
       </c>

</xml_diff>